<commit_message>
Updated data and build commands
</commit_message>
<xml_diff>
--- a/data/SuperEndpoint Mapping 2020Sept2.xlsx
+++ b/data/SuperEndpoint Mapping 2020Sept2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23219"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/sara_gosline_pnnl_gov/Documents/Documents/BitBucket/SRPDataVis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gosl241\OneDrive - PNNL\Documents\GitHub\srpAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="265" documentId="8_{173A47B2-8EA1-4EEB-A1E2-29452B2FC89C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C5E8DFB2-5466-4593-83C7-7FE39CD7D680}"/>
+  <xr:revisionPtr revIDLastSave="299" documentId="8_{173A47B2-8EA1-4EEB-A1E2-29452B2FC89C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{77CBF66E-0ECC-46A5-A45E-882180620802}"/>
   <bookViews>
-    <workbookView xWindow="-27735" yWindow="1980" windowWidth="11280" windowHeight="13515" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30555" yWindow="3180" windowWidth="21600" windowHeight="12675" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="205">
   <si>
     <t>New Endpoints</t>
   </si>
@@ -599,13 +599,58 @@
   </si>
   <si>
     <t>LTKR</t>
+  </si>
+  <si>
+    <t>Ontology Link</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UBERON_0000071</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ZP_0005012</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ZP_0000305</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ZP_0015467</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ZP_0000624</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ZP_0003437 | http://purl.obolibrary.org/obo/ZP_0010405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/ZP_0001225 | http://purl.obolibrary.org/obo/ZP_0020238 | http://purl.obolibrary.org/obo/ZP_0000011 </t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ZP_0000943 | http://purl.obolibrary.org/obo/ZP_0014550 | http://purl.obolibrary.org/obo/ZP_0007203</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ZP_0001601 | http://purl.obolibrary.org/obo/ZP_0000100 | http://purl.obolibrary.org/obo/ZP_0008625</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/ZP_0002060 | </t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ZP_0009084</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ZP_0100440</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ZP_0012599</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ZP_0137685</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -617,6 +662,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -680,10 +733,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -701,8 +755,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1620,10 +1677,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0498EF9C-E9A3-468C-A290-DEE17D385575}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1631,9 +1688,10 @@
     <col min="1" max="1" width="13.77734375" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" customWidth="1"/>
     <col min="3" max="3" width="74.21875" customWidth="1"/>
+    <col min="4" max="4" width="119.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1643,19 +1701,22 @@
       <c r="C1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>185</v>
       </c>
@@ -1666,29 +1727,32 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>58</v>
+        <v>188</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
@@ -1698,8 +1762,11 @@
       <c r="C6" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>187</v>
       </c>
@@ -1709,8 +1776,11 @@
       <c r="C7" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>15</v>
       </c>
@@ -1720,152 +1790,201 @@
       <c r="C8" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="D10" s="11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="D11" s="12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B15" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C15" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="D15" s="12" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>181</v>
+      </c>
+      <c r="D16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17" t="s">
+        <v>183</v>
+      </c>
+      <c r="D17" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B18" t="s">
         <v>32</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C18" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="D18" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
+        <v>184</v>
+      </c>
+      <c r="D19" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B20" t="s">
         <v>35</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C20" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" t="s">
-        <v>182</v>
-      </c>
-      <c r="C15" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>188</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>73</v>
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D21">
+    <sortCondition ref="A2:A21"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{85B8E2B7-BBE9-41E6-AF99-87FC8ACEA738}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2124,21 +2243,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100396ED2E7A640164CB8C59FDEC2C765CC" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="26e8590940edae28bea0b080f6fa8b06">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7a9331905dac936d9e88b896f6b901d6" ns3:_="">
     <xsd:import namespace="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3"/>
@@ -2308,31 +2412,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{565D9DA6-2D7C-4976-B32E-584E4A2A7F7C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E57FCB-AF0B-40B5-9F88-8BBFA3B90FEE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8D080FC-E009-4447-ACD6-B9CB0ED3D7DD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2348,4 +2443,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E57FCB-AF0B-40B5-9F88-8BBFA3B90FEE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{565D9DA6-2D7C-4976-B32E-584E4A2A7F7C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
moved files around to clean up top level directory
</commit_message>
<xml_diff>
--- a/data/SuperEndpoint Mapping 2020Sept2.xlsx
+++ b/data/SuperEndpoint Mapping 2020Sept2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gosl241\OneDrive - PNNL\Documents\GitHub\srpAnalytics\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/sara_gosline_pnnl_gov/Documents/Documents/GitHub/srpAnalytics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="299" documentId="8_{173A47B2-8EA1-4EEB-A1E2-29452B2FC89C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{77CBF66E-0ECC-46A5-A45E-882180620802}"/>
+  <xr:revisionPtr revIDLastSave="303" documentId="8_{173A47B2-8EA1-4EEB-A1E2-29452B2FC89C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4ED552C3-1AA7-48F3-A4FA-7AECB039E1FC}"/>
   <bookViews>
-    <workbookView xWindow="30555" yWindow="3180" windowWidth="21600" windowHeight="12675" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30720" yWindow="1920" windowWidth="17610" windowHeight="13005" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="204">
   <si>
     <t>New Endpoints</t>
   </si>
@@ -205,9 +205,6 @@
     <t>TOT_MORT</t>
   </si>
   <si>
-    <t>ANY_MORT</t>
-  </si>
-  <si>
     <t>MOV1</t>
   </si>
   <si>
@@ -598,9 +595,6 @@
     <t>AUC1</t>
   </si>
   <si>
-    <t>LTKR</t>
-  </si>
-  <si>
     <t>Ontology Link</t>
   </si>
   <si>
@@ -644,6 +638,9 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/ZP_0137685</t>
+  </si>
+  <si>
+    <t>ALL_BUT_MORT</t>
   </si>
 </sst>
 </file>
@@ -752,11 +749,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1122,13 +1119,13 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1136,10 +1133,10 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1147,10 +1144,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
         <v>86</v>
-      </c>
-      <c r="C3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1158,10 +1155,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
         <v>88</v>
-      </c>
-      <c r="C4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1169,21 +1166,21 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
         <v>90</v>
-      </c>
-      <c r="C5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1191,21 +1188,21 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1213,10 +1210,10 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" t="s">
         <v>99</v>
-      </c>
-      <c r="C9" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1224,43 +1221,43 @@
         <v>29</v>
       </c>
       <c r="B10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" t="s">
         <v>101</v>
-      </c>
-      <c r="C10" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
         <v>104</v>
-      </c>
-      <c r="C12" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1268,10 +1265,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1279,43 +1276,43 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" t="s">
         <v>113</v>
-      </c>
-      <c r="C15" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" t="s">
         <v>115</v>
-      </c>
-      <c r="C16" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1323,43 +1320,43 @@
         <v>30</v>
       </c>
       <c r="B19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" t="s">
         <v>119</v>
-      </c>
-      <c r="C19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" t="s">
         <v>121</v>
-      </c>
-      <c r="C20" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" t="s">
         <v>124</v>
-      </c>
-      <c r="C22" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1393,11 +1390,11 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1680,7 +1677,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1696,35 +1693,35 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>58</v>
+        <v>203</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1732,24 +1729,24 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1760,24 +1757,24 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1788,10 +1785,10 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1799,13 +1796,13 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1816,24 +1813,24 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>138</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>200</v>
+        <v>137</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>189</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>139</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>196</v>
+        <v>138</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1841,13 +1838,13 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1858,24 +1855,24 @@
         <v>43</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1886,38 +1883,38 @@
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>140</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>197</v>
+        <v>139</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B16" t="s">
         <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C17" t="s">
         <v>182</v>
       </c>
-      <c r="C17" t="s">
-        <v>183</v>
-      </c>
       <c r="D17" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1928,10 +1925,10 @@
         <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1939,13 +1936,13 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1956,10 +1953,10 @@
         <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D20" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1967,13 +1964,13 @@
         <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2007,35 +2004,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2043,10 +2040,10 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -2054,43 +2051,43 @@
         <v>29</v>
       </c>
       <c r="B5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" t="s">
         <v>147</v>
-      </c>
-      <c r="C5" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" t="s">
         <v>150</v>
-      </c>
-      <c r="C7" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" t="s">
         <v>153</v>
-      </c>
-      <c r="C8" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -2098,7 +2095,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -2106,43 +2103,43 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C11" t="s">
         <v>172</v>
-      </c>
-      <c r="C11" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -2150,52 +2147,52 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C14" t="s">
         <v>157</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
         <v>158</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>159</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>160</v>
-      </c>
-      <c r="G14" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B15" t="s">
+        <v>175</v>
+      </c>
+      <c r="C15" t="s">
         <v>176</v>
-      </c>
-      <c r="C15" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C17" t="s">
         <v>162</v>
-      </c>
-      <c r="C17" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -2203,38 +2200,38 @@
         <v>39</v>
       </c>
       <c r="B18" t="s">
+        <v>173</v>
+      </c>
+      <c r="C18" t="s">
         <v>174</v>
-      </c>
-      <c r="C18" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>164</v>
+      </c>
+      <c r="B19" t="s">
         <v>165</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>166</v>
       </c>
-      <c r="C19" t="s">
-        <v>167</v>
-      </c>
       <c r="E19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B20" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" t="s">
         <v>168</v>
       </c>
-      <c r="C20" t="s">
-        <v>169</v>
-      </c>
       <c r="E20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2243,6 +2240,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100396ED2E7A640164CB8C59FDEC2C765CC" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="26e8590940edae28bea0b080f6fa8b06">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7a9331905dac936d9e88b896f6b901d6" ns3:_="">
     <xsd:import namespace="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3"/>
@@ -2412,22 +2424,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{565D9DA6-2D7C-4976-B32E-584E4A2A7F7C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E57FCB-AF0B-40B5-9F88-8BBFA3B90FEE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8D080FC-E009-4447-ACD6-B9CB0ED3D7DD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2443,28 +2464,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E57FCB-AF0B-40B5-9F88-8BBFA3B90FEE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{565D9DA6-2D7C-4976-B32E-584E4A2A7F7C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>